<commit_message>
Add: Add one more column
Add one more column.

Signed-off-by: @surajgirioffl
</commit_message>
<xml_diff>
--- a/preferences.xlsx
+++ b/preferences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Freelancing\Real Development\Web Scraping And Browser Automation\01 - AITINC\02 - AI Generators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ADFB2C-E13F-41B3-BD68-96219C5E78B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C935BBAC-612A-4C53-8D92-77E0D069AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="21600" windowHeight="14380" xr2:uid="{EE29AFC5-2453-45A0-8F9F-EDFA065A8214}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{EE29AFC5-2453-45A0-8F9F-EDFA065A8214}"/>
   </bookViews>
   <sheets>
     <sheet name="options" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>pixverse</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>site</t>
+  </si>
+  <si>
+    <t>login_required</t>
   </si>
 </sst>
 </file>
@@ -597,11 +600,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3575C387-9627-498B-85E5-2E5CD3DD0826}">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,21 +612,22 @@
     <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -634,67 +638,70 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -704,32 +711,35 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="X2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="Y2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -739,35 +749,38 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="X3" s="3"/>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="Y3" s="3"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -777,21 +790,24 @@
       <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -801,21 +817,24 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -825,18 +844,21 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -846,21 +868,24 @@
       <c r="C7" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -870,26 +895,29 @@
       <c r="C8" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: Add some sample sheets
Add some sample sheets.

Signed-off-by: @surajgirioffl
</commit_message>
<xml_diff>
--- a/preferences.xlsx
+++ b/preferences.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Freelancing\Real Development\Web Scraping And Browser Automation\01 - AITINC\02 - AI Generators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C935BBAC-612A-4C53-8D92-77E0D069AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CB56FF-C488-45C2-87D6-622596B006AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{EE29AFC5-2453-45A0-8F9F-EDFA065A8214}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="5" xr2:uid="{EE29AFC5-2453-45A0-8F9F-EDFA065A8214}"/>
   </bookViews>
   <sheets>
     <sheet name="options" sheetId="1" r:id="rId1"/>
-    <sheet name="prompts" sheetId="2" r:id="rId2"/>
+    <sheet name="prompts1" sheetId="2" r:id="rId2"/>
+    <sheet name="prompts2" sheetId="3" r:id="rId3"/>
+    <sheet name="prompts3" sheetId="4" r:id="rId4"/>
+    <sheet name="prompts4" sheetId="5" r:id="rId5"/>
+    <sheet name="images1" sheetId="6" r:id="rId6"/>
+    <sheet name="images2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>pixverse</t>
   </si>
@@ -602,9 +607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3575C387-9627-498B-85E5-2E5CD3DD0826}">
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,7 +937,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,4 +965,119 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00A4CC1-D2B9-4C55-A973-AA4756DE3435}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F51E55-BA9A-4EC0-9C0C-FE52830E9043}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5D2337-63AA-4B1F-89D2-B05694E0AC14}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBF1925-306D-444B-9797-AB006461F109}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9744A689-66BF-48EB-BB9D-45141A8EB597}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove: Remove default provided prompt
Remove default provided prompt from a prompt sheet.

Signed-off-by: @surajgirioffl
</commit_message>
<xml_diff>
--- a/preferences.xlsx
+++ b/preferences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Freelancing\Real Development\Web Scraping And Browser Automation\01 - AITINC\02 - AI Generators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CB56FF-C488-45C2-87D6-622596B006AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8503BC-E3DE-49C7-88A5-1C94EE04985D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="5" xr2:uid="{EE29AFC5-2453-45A0-8F9F-EDFA065A8214}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="1" xr2:uid="{EE29AFC5-2453-45A0-8F9F-EDFA065A8214}"/>
   </bookViews>
   <sheets>
     <sheet name="options" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>pixverse</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>sno</t>
-  </si>
-  <si>
-    <t>Create a video showcasing a tranquil waterfall surrounded by lush greenery, with sunlight filtering through the trees and birds chirping in the background. Include close-up shots of colorful flowers blooming and butterflies fluttering around. The scene should evoke a sense of peace and serenity</t>
   </si>
   <si>
     <t>site</t>
@@ -609,7 +606,7 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +631,7 @@
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>37</v>
@@ -643,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -936,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897D2818-D90E-42B5-A441-FFA2C04F7FD4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -954,13 +951,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>52</v>
-      </c>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -972,7 +964,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBF1925-306D-444B-9797-AB006461F109}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>